<commit_message>
changes from work comp
</commit_message>
<xml_diff>
--- a/app/recipes.xlsx
+++ b/app/recipes.xlsx
@@ -230,9 +230,6 @@
     <t>Lunch | Dinner | Side</t>
   </si>
   <si>
-    <t>Corn &amp; Jalapeno Ho Cakes</t>
-  </si>
-  <si>
     <t>corn_and_jalapeno_ho_cakes</t>
   </si>
   <si>
@@ -317,9 +314,6 @@
     <t>peanut_chicken_salad</t>
   </si>
   <si>
-    <t>Short Ribs Lettuce Wraps</t>
-  </si>
-  <si>
     <t>short_ribs_lettuce_wraps</t>
   </si>
   <si>
@@ -623,9 +617,6 @@
     <t>BrsdPrkRstdRtVgtblsFrtCmpt.pdf</t>
   </si>
   <si>
-    <t>CrnJlpnHoCakes.pdf</t>
-  </si>
-  <si>
     <t>CrrdClflwr.pdf</t>
   </si>
   <si>
@@ -686,9 +677,6 @@
     <t>StrwvcdSmthie.pdf</t>
   </si>
   <si>
-    <t>ShrtRibLettuceWraps.pdf</t>
-  </si>
-  <si>
     <t>ShrimpTacos.pdf</t>
   </si>
   <si>
@@ -708,6 +696,18 @@
   </si>
   <si>
     <t>StrawberryAvoSmoothieThumbnail.jpg</t>
+  </si>
+  <si>
+    <t>Corn &amp; Jalapeno Hoe Cakes</t>
+  </si>
+  <si>
+    <t>CrnJlpnHoeCakes.pdf</t>
+  </si>
+  <si>
+    <t>Short Ribs Lettuce Cups</t>
+  </si>
+  <si>
+    <t>ShrtRibLettuceCups.pdf</t>
   </si>
 </sst>
 </file>
@@ -1087,7 +1087,7 @@
   <dimension ref="A1:K38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1115,7 +1115,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>3</v>
@@ -1147,19 +1147,19 @@
         <v>42</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E2" s="5">
         <v>2</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="H2" s="5" t="s">
         <v>43</v>
@@ -1178,19 +1178,19 @@
         <v>46</v>
       </c>
       <c r="C3" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="D3" s="8" t="s">
         <v>146</v>
       </c>
-      <c r="D3" s="8" t="s">
-        <v>148</v>
-      </c>
       <c r="E3" s="8">
         <v>1</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="H3" s="8" t="s">
         <v>47</v>
@@ -1209,19 +1209,19 @@
         <v>50</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="E4" s="5">
         <v>1</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="H4" s="5" t="s">
         <v>21</v>
@@ -1240,19 +1240,19 @@
         <v>53</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="E5" s="5">
         <v>1</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="H5" s="5" t="s">
         <v>54</v>
@@ -1271,19 +1271,19 @@
         <v>57</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E6" s="5">
         <v>1</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="H6" s="5" t="s">
         <v>43</v>
@@ -1302,19 +1302,19 @@
         <v>59</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="E7" s="5">
         <v>1</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="H7" s="5" t="s">
         <v>43</v>
@@ -1333,19 +1333,19 @@
         <v>62</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E8" s="5">
         <v>2</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="H8" s="5" t="s">
         <v>47</v>
@@ -1364,19 +1364,19 @@
         <v>64</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="E9" s="5">
         <v>1</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="H9" s="5" t="s">
         <v>65</v>
@@ -1389,59 +1389,59 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
+        <v>222</v>
+      </c>
+      <c r="B10" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="C10" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="E10" s="5">
+        <v>1</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>223</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="H10" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="C10" s="5" t="s">
-        <v>161</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>162</v>
-      </c>
-      <c r="E10" s="5">
-        <v>1</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>197</v>
-      </c>
-      <c r="G10" s="4" t="s">
-        <v>132</v>
-      </c>
-      <c r="H10" s="5" t="s">
+      <c r="I10" s="4" t="s">
         <v>68</v>
-      </c>
-      <c r="I10" s="4" t="s">
-        <v>69</v>
       </c>
       <c r="J10" s="4"/>
       <c r="K10" s="4"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="B11" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="C11" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="E11" s="5">
+        <v>1</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="H11" s="5" t="s">
         <v>71</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>163</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>164</v>
-      </c>
-      <c r="E11" s="5">
-        <v>1</v>
-      </c>
-      <c r="F11" s="5" t="s">
-        <v>199</v>
-      </c>
-      <c r="G11" s="4" t="s">
-        <v>132</v>
-      </c>
-      <c r="H11" s="5" t="s">
-        <v>72</v>
       </c>
       <c r="I11" s="4" t="s">
         <v>44</v>
@@ -1451,87 +1451,87 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="B12" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="B12" s="5" t="s">
-        <v>74</v>
-      </c>
       <c r="C12" s="5" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="E12" s="5">
         <v>1</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="H12" s="5" t="s">
         <v>43</v>
       </c>
       <c r="I12" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J12" s="4"/>
       <c r="K12" s="4"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="B13" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="C13" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="E13" s="5">
+        <v>1</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="H13" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="C13" s="5" t="s">
-        <v>166</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>167</v>
-      </c>
-      <c r="E13" s="5">
-        <v>1</v>
-      </c>
-      <c r="F13" s="5" t="s">
-        <v>209</v>
-      </c>
-      <c r="G13" s="4" t="s">
-        <v>132</v>
-      </c>
-      <c r="H13" s="5" t="s">
+      <c r="I13" s="4" t="s">
         <v>78</v>
-      </c>
-      <c r="I13" s="4" t="s">
-        <v>79</v>
       </c>
       <c r="J13" s="4"/>
       <c r="K13" s="4"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E14" s="5">
         <v>2</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="H14" s="5" t="s">
         <v>47</v>
@@ -1544,25 +1544,25 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E15" s="5">
         <v>1</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="H15" s="5" t="s">
         <v>47</v>
@@ -1575,59 +1575,59 @@
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="B16" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="B16" s="5" t="s">
-        <v>81</v>
-      </c>
       <c r="C16" s="5" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E16" s="5">
         <v>1</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="H16" s="5" t="s">
         <v>47</v>
       </c>
       <c r="I16" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J16" s="4"/>
       <c r="K16" s="4"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="B17" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="B17" s="5" t="s">
-        <v>84</v>
-      </c>
       <c r="C17" s="5" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="E17" s="5">
         <v>2</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="H17" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="I17" s="4" t="s">
         <v>48</v>
@@ -1637,56 +1637,56 @@
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="B18" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="B18" s="5" t="s">
-        <v>87</v>
-      </c>
       <c r="C18" s="5" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="E18" s="5">
         <v>1</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="H18" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="I18" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J18" s="4"/>
       <c r="K18" s="4"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="B19" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="B19" s="5" t="s">
-        <v>89</v>
-      </c>
       <c r="C19" s="5" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="E19" s="5">
         <v>1</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="H19" s="5" t="s">
         <v>43</v>
@@ -1699,28 +1699,28 @@
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="B20" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="B20" s="5" t="s">
-        <v>91</v>
-      </c>
       <c r="C20" s="5" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="E20" s="5">
         <v>2</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="G20" s="4" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="H20" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="I20" s="4" t="s">
         <v>44</v>
@@ -1730,28 +1730,28 @@
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="B21" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="B21" s="5" t="s">
-        <v>94</v>
-      </c>
       <c r="C21" s="5" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="E21" s="5">
         <v>1</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="H21" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="I21" s="4" t="s">
         <v>44</v>
@@ -1761,28 +1761,28 @@
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" s="5" t="s">
+        <v>224</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="E22" s="5">
+        <v>1</v>
+      </c>
+      <c r="F22" s="5" t="s">
+        <v>225</v>
+      </c>
+      <c r="G22" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="H22" s="5" t="s">
         <v>95</v>
-      </c>
-      <c r="B22" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="C22" s="5" t="s">
-        <v>176</v>
-      </c>
-      <c r="D22" s="5" t="s">
-        <v>177</v>
-      </c>
-      <c r="E22" s="5">
-        <v>1</v>
-      </c>
-      <c r="F22" s="5" t="s">
-        <v>218</v>
-      </c>
-      <c r="G22" s="4" t="s">
-        <v>132</v>
-      </c>
-      <c r="H22" s="5" t="s">
-        <v>97</v>
       </c>
       <c r="I22" s="4" t="s">
         <v>44</v>
@@ -1792,279 +1792,279 @@
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" s="5" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E23" s="5">
         <v>1</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="G23" s="4" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="H23" s="5" t="s">
         <v>43</v>
       </c>
       <c r="I23" s="4" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="J23" s="4"/>
       <c r="K23" s="4"/>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="E24" s="5">
         <v>1</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="G24" s="4" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="H24" s="5" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="I24" s="4" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="J24" s="4"/>
       <c r="K24" s="4"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" s="5" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="E25" s="5">
         <v>1</v>
       </c>
       <c r="F25" s="5" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="G25" s="4" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="H25" s="5" t="s">
         <v>43</v>
       </c>
       <c r="I25" s="4" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="J25" s="4"/>
       <c r="K25" s="4"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" s="5" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="E26" s="5">
         <v>1</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="G26" s="4" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="H26" s="5" t="s">
         <v>43</v>
       </c>
       <c r="I26" s="4" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="J26" s="4"/>
       <c r="K26" s="4"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27" s="5" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="E27" s="5">
         <v>1</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="G27" s="4" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="H27" s="5" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="I27" s="4" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="J27" s="4"/>
       <c r="K27" s="4"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28" s="5" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="E28" s="5">
         <v>1</v>
       </c>
       <c r="F28" s="5" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="G28" s="4" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="H28" s="5" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="I28" s="4" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="J28" s="4"/>
       <c r="K28" s="4"/>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29" s="5" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C29" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="D29" s="5" t="s">
         <v>149</v>
-      </c>
-      <c r="D29" s="5" t="s">
-        <v>151</v>
       </c>
       <c r="E29" s="5">
         <v>2</v>
       </c>
       <c r="F29" s="5" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="G29" s="4" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="H29" s="5" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="I29" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J29" s="4"/>
       <c r="K29" s="4"/>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A30" s="5" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C30" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="D30" s="5" t="s">
         <v>150</v>
       </c>
-      <c r="D30" s="5" t="s">
-        <v>152</v>
-      </c>
       <c r="E30" s="5">
         <v>1</v>
       </c>
       <c r="F30" s="5" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="G30" s="4" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="H30" s="5" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="I30" s="4" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="J30" s="4"/>
       <c r="K30" s="4"/>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A31" s="5" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="E31" s="5">
         <v>1</v>
       </c>
       <c r="F31" s="5" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="G31" s="4" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="H31" s="5" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="I31" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J31" s="4"/>
       <c r="K31" s="4"/>
@@ -2080,16 +2080,16 @@
         <v>27</v>
       </c>
       <c r="D32" s="8" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="E32" s="5">
         <v>1</v>
       </c>
       <c r="F32" s="4" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="G32" s="4" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="H32" s="8" t="s">
         <v>28</v>
@@ -2111,16 +2111,16 @@
         <v>12</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="E33" s="5">
         <v>1</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="G33" s="4" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="H33" s="5" t="s">
         <v>13</v>
@@ -2142,16 +2142,16 @@
         <v>24</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="E34" s="5">
         <v>1</v>
       </c>
       <c r="F34" s="5" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="G34" s="4" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="H34" s="5" t="s">
         <v>18</v>
@@ -2173,16 +2173,16 @@
         <v>17</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="E35" s="5">
         <v>1</v>
       </c>
       <c r="F35" s="4" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="G35" s="4" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="H35" s="5" t="s">
         <v>18</v>
@@ -2204,16 +2204,16 @@
         <v>35</v>
       </c>
       <c r="D36" s="7" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="E36" s="5">
         <v>1</v>
       </c>
       <c r="F36" s="7" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="G36" s="4" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="H36" s="8" t="s">
         <v>43</v>
@@ -2235,16 +2235,16 @@
         <v>36</v>
       </c>
       <c r="D37" s="7" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="E37" s="5">
         <v>2</v>
       </c>
       <c r="F37" s="7" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="G37" s="4" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="H37" s="8" t="s">
         <v>43</v>
@@ -2266,19 +2266,19 @@
         <v>37</v>
       </c>
       <c r="D38" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E38" s="5">
         <v>1</v>
       </c>
       <c r="F38" s="7" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="G38" s="4" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="H38" s="8" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="I38" s="7" t="s">
         <v>40</v>

</xml_diff>